<commit_message>
New updates to main page, committing edits that were previously published but not uploaded to git.
</commit_message>
<xml_diff>
--- a/agquery/Update/Policy_Pathways.xlsx
+++ b/agquery/Update/Policy_Pathways.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanisha4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED856344-0656-4298-9617-2B6205D5E54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB12541-AFFC-4A54-B056-5DC7EB8F2F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{72E42A8E-C175-46F8-A795-34B91AF3F2A6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{72E42A8E-C175-46F8-A795-34B91AF3F2A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy_Pathways _ APN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="140">
   <si>
     <t>pathwayID</t>
   </si>
@@ -818,6 +818,18 @@
       </rPr>
       <t>(4), e406-e422.</t>
     </r>
+  </si>
+  <si>
+    <t>Promote Seed Industry and Management of Agricultural Inputs</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Strengthen Agricultural Extension</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1389,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1387,7 +1399,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1764,1504 +1775,1524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D25450-242E-4EDD-AF00-8EC17FCB4AD4}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="7"/>
-    <col min="3" max="3" width="27.06640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="70.9296875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.59765625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="70.265625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="7"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="71" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2" s="7">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="7">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="7" t="s">
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="7">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="J4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="7">
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K5" s="7" t="s">
+      <c r="G5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="7" t="s">
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="7">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="7">
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="H8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="7" t="s">
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" s="7">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="H9" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="J9" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="7">
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" s="7" t="s">
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="7" t="s">
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="7">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K11" s="7" t="s">
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="7">
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K12" s="7" t="s">
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="7" t="s">
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="7">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="7">
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>129</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K14" s="7" t="s">
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="7" t="s">
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" s="7">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="H15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="7" t="s">
+      <c r="L15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A16" s="7">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="7" t="s">
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A17" s="7">
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" t="s">
         <v>93</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="7" t="s">
+      <c r="L17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="7">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="7">
+      <c r="L18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="7" t="s">
+      <c r="L19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="H20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="7">
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" t="s">
         <v>93</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="I21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="7" t="s">
+      <c r="L21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="7">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" t="s">
         <v>93</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K22" s="7" t="s">
+      <c r="J22" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="7">
+      <c r="L22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K23" s="7" t="s">
+      <c r="H23" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" t="s">
         <v>34</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="7">
+      <c r="L23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K24" s="7" t="s">
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
         <v>34</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="7" t="s">
+      <c r="L24" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="7">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" s="7" t="s">
+      <c r="H25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="7" t="s">
+      <c r="L25" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A26" s="7">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="7" t="s">
+      <c r="H26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A27" s="7">
+      <c r="L26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K27" s="7" t="s">
+      <c r="H27" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" t="s">
         <v>23</v>
       </c>
-      <c r="L27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="7" t="s">
+      <c r="L27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A28" s="7">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K28" s="7" t="s">
+      <c r="J28" t="s">
+        <v>92</v>
+      </c>
+      <c r="K28" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="7">
+      <c r="L28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="7" t="s">
+      <c r="I29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="7" t="s">
+      <c r="L29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A30" s="7">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K30" s="7" t="s">
+      <c r="I30" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" t="s">
         <v>18</v>
       </c>
-      <c r="L30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="7" t="s">
+      <c r="L30" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A31" s="7">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K31" s="7" t="s">
+      <c r="I31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" t="s">
         <v>23</v>
       </c>
-      <c r="L31" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="7" t="s">
+      <c r="L31" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A32" s="7">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K32" s="7" t="s">
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" t="s">
         <v>34</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="7" t="s">
+      <c r="L32" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33" s="7">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K33" s="7" t="s">
+      <c r="H33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" t="s">
         <v>23</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="7" t="s">
+      <c r="L33" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34" s="7">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" t="s">
         <v>27</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K34" s="7" t="s">
+      <c r="H34" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" t="s">
+        <v>91</v>
+      </c>
+      <c r="J34" t="s">
+        <v>91</v>
+      </c>
+      <c r="K34" t="s">
         <v>23</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="7" t="s">
+      <c r="L34" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35" s="7">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" t="s">
         <v>93</v>
       </c>
-      <c r="I35" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K35" s="7" t="s">
+      <c r="I35" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" t="s">
         <v>23</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" s="7" t="s">
+      <c r="L35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A36" s="7">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" t="s">
         <v>94</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K36" s="7" t="s">
+      <c r="G36" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" t="s">
         <v>23</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="7" t="s">
+      <c r="L36" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A37" s="7">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K37" s="7" t="s">
+      <c r="G37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" t="s">
+        <v>91</v>
+      </c>
+      <c r="I37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" t="s">
+        <v>92</v>
+      </c>
+      <c r="K37" t="s">
         <v>34</v>
       </c>
-      <c r="L37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="7" t="s">
+      <c r="L37" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3273,17 +3304,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8B157-5ECB-435B-A7A7-C0C9DF850AED}">
   <dimension ref="A2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>105</v>
       </c>
@@ -3297,7 +3328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -3310,7 +3341,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
@@ -3324,7 +3355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="114" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>111</v>
       </c>
@@ -3338,7 +3369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>114</v>
       </c>
@@ -3352,7 +3383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>100</v>
       </c>
@@ -3366,7 +3397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>117</v>
       </c>
@@ -3379,7 +3410,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>118</v>
       </c>
@@ -3393,7 +3424,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>121</v>
       </c>
@@ -3407,7 +3438,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>124</v>
       </c>
@@ -3421,7 +3452,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Release cleanup and bug fixes, extensions to the documentation. Substantial reorganization and cleanup of main app file to reduce unnecessary code/undo some hard coding performed for demo.
</commit_message>
<xml_diff>
--- a/agquery/Update/Policy_Pathways.xlsx
+++ b/agquery/Update/Policy_Pathways.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4930468-FBE0-4403-94BB-6245ABE95521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4802CAD0-2A39-4D7F-B94C-C6E9C24E3E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{BF764781-96BE-4222-A64E-0AD10A526D8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF764781-96BE-4222-A64E-0AD10A526D8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy_Pathways" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="97">
   <si>
     <t>pathwayID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>goalName</t>
   </si>
   <si>
-    <t>Policy.Goal</t>
-  </si>
-  <si>
     <t>Pathway</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Poultry</t>
   </si>
   <si>
-    <t>Improve domestic poultry production &amp; consumption</t>
-  </si>
-  <si>
     <t>Reduce Producer Feed Cost</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t>Livestock</t>
   </si>
   <si>
-    <t>Reduce imports of beef by increasing domestic production</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reduce producer feed cost </t>
   </si>
   <si>
@@ -320,9 +311,6 @@
   </si>
   <si>
     <t>Cashews</t>
-  </si>
-  <si>
-    <t>Improve Cashew Producer Income</t>
   </si>
 </sst>
 </file>
@@ -1183,13 +1171,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54DF1CC-871D-4F8B-92EA-DC1DD07E9EFB}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="103" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,1536 +1223,1419 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
       <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="L4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
       <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>20</v>
-      </c>
       <c r="K10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
       <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
         <v>16</v>
       </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
       <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
-        <v>58</v>
-      </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s">
         <v>19</v>
       </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
       <c r="K16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
       <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J17" t="s">
         <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
         <v>63</v>
       </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
         <v>64</v>
       </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
         <v>16</v>
       </c>
-      <c r="F21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
       <c r="H22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" t="s">
-        <v>71</v>
-      </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" t="s">
         <v>19</v>
       </c>
-      <c r="I23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" t="s">
-        <v>20</v>
-      </c>
       <c r="K23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L23" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L25" t="s">
-        <v>22</v>
-      </c>
-      <c r="M25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L26" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K27" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L27" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
         <v>16</v>
       </c>
-      <c r="F29" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" t="s">
-        <v>36</v>
-      </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I29" t="s">
         <v>18</v>
       </c>
       <c r="J29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L29" t="s">
-        <v>22</v>
-      </c>
-      <c r="M29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K30" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L30" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="F31" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="G31" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" t="s">
         <v>19</v>
       </c>
-      <c r="J31" t="s">
-        <v>20</v>
-      </c>
       <c r="K31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L31" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="D32" t="s">
-        <v>87</v>
-      </c>
       <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
         <v>16</v>
       </c>
-      <c r="F32" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" t="s">
-        <v>36</v>
-      </c>
       <c r="H32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L32" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="D33" t="s">
-        <v>87</v>
-      </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L33" t="s">
-        <v>22</v>
-      </c>
-      <c r="M33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J34" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K34" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>22</v>
-      </c>
-      <c r="M34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K35" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" t="s">
         <v>16</v>
       </c>
-      <c r="F36" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" t="s">
-        <v>36</v>
-      </c>
       <c r="H36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J36" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K36" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L36" t="s">
-        <v>22</v>
-      </c>
-      <c r="M36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J37" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K37" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>22</v>
-      </c>
-      <c r="M38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>